<commit_message>
Suspected Location column changed to Location
</commit_message>
<xml_diff>
--- a/eleusis_master.xlsx
+++ b/eleusis_master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13120"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13120" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Inscription" sheetId="1" r:id="rId1"/>
@@ -17,11 +17,11 @@
     <sheet name="Institution" sheetId="2" r:id="rId3"/>
     <sheet name="Person" sheetId="3" r:id="rId4"/>
     <sheet name="Honor" sheetId="4" r:id="rId5"/>
-    <sheet name="Institution Sponsor" sheetId="5" r:id="rId6"/>
+    <sheet name="Institution Sponsorship" sheetId="5" r:id="rId6"/>
     <sheet name="Institution Honor" sheetId="6" r:id="rId7"/>
     <sheet name="Honor in Inscription" sheetId="7" r:id="rId8"/>
     <sheet name="Person in Inscription" sheetId="13" r:id="rId9"/>
-    <sheet name="Person Displaying Honor" sheetId="8" r:id="rId10"/>
+    <sheet name="Person Honor Display" sheetId="8" r:id="rId10"/>
     <sheet name="Personal Relationship" sheetId="18" r:id="rId11"/>
     <sheet name="Inscription Macroscopic" sheetId="16" r:id="rId12"/>
     <sheet name="Multistone Inscription" sheetId="17" r:id="rId13"/>
@@ -8351,7 +8351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M427"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -23581,8 +23581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E518"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E398" sqref="E398"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
column name correction on eleusis_master
</commit_message>
<xml_diff>
--- a/eleusis_master.xlsx
+++ b/eleusis_master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="13125" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="13125" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Inscription" sheetId="1" r:id="rId1"/>
@@ -32,19 +32,17 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13495" uniqueCount="2434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13495" uniqueCount="2435">
   <si>
     <t>Statue Base for an Unknown Kanephoros</t>
   </si>
@@ -7359,6 +7357,9 @@
   </si>
   <si>
     <t>190</t>
+  </si>
+  <si>
+    <t>Institution</t>
   </si>
 </sst>
 </file>
@@ -8176,7 +8177,7 @@
   <autoFilter ref="A1:F26"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Name"/>
+    <tableColumn id="2" name="Institution"/>
     <tableColumn id="3" name="Origin"/>
     <tableColumn id="4" name="Type"/>
     <tableColumn id="5" name="Category"/>
@@ -32639,12 +32640,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K680"/>
   <sheetViews>
-    <sheetView topLeftCell="A427" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="B197" sqref="B197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="105.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
@@ -50686,8 +50688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A486" workbookViewId="0">
-      <selection activeCell="F510" sqref="F510"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K502" sqref="K502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64179,8 +64181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64193,7 +64195,7 @@
         <v>1238</v>
       </c>
       <c r="B1" t="s">
-        <v>1244</v>
+        <v>2434</v>
       </c>
       <c r="C1" t="s">
         <v>1234</v>

</xml_diff>

<commit_message>
macroscopic field 'title' changed to 'institution'
</commit_message>
<xml_diff>
--- a/eleusis_master.xlsx
+++ b/eleusis_master.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="13125" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="13125" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Inscription" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13495" uniqueCount="2435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13495" uniqueCount="2436">
   <si>
     <t>Statue Base for an Unknown Kanephoros</t>
   </si>
@@ -7360,6 +7359,9 @@
   </si>
   <si>
     <t>Institution</t>
+  </si>
+  <si>
+    <t>Inscription</t>
   </si>
 </sst>
 </file>
@@ -8114,7 +8116,7 @@
   <autoFilter ref="A1:K680"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Title"/>
+    <tableColumn id="2" name="Inscription"/>
     <tableColumn id="3" name="Date"/>
     <tableColumn id="4" name="Date Strength"/>
     <tableColumn id="5" name="Inscription Type"/>
@@ -23780,7 +23782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E518"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
@@ -32640,8 +32642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K680"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="B197" sqref="B197"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32662,7 +32664,7 @@
         <v>1238</v>
       </c>
       <c r="B1" t="s">
-        <v>1246</v>
+        <v>2435</v>
       </c>
       <c r="C1" t="s">
         <v>1251</v>
@@ -64181,7 +64183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -64647,7 +64649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P540"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="Q431" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
workbork re-converted to tables
</commit_message>
<xml_diff>
--- a/eleusis_master.xlsx
+++ b/eleusis_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidthomas/Git/brown-diss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA26EFE-F259-3743-A2EA-B44938117870}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19514AE1-6108-6741-A801-8ED774899DB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0C2D7FDC-D2BD-754C-9966-FCA1A3DC457F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="12" xr2:uid="{0C2D7FDC-D2BD-754C-9966-FCA1A3DC457F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inscription" sheetId="1" r:id="rId1"/>
@@ -27,21 +27,6 @@
     <sheet name="Person in Inscription" sheetId="12" r:id="rId12"/>
     <sheet name="Person Honor Display" sheetId="13" r:id="rId13"/>
   </sheets>
-  <definedNames>
-    <definedName name="Honor" localSheetId="3">Honor!$A$1:$F$141</definedName>
-    <definedName name="Honor_in_Inscription" localSheetId="8">'Honor in Inscription'!$A$1:$D$492</definedName>
-    <definedName name="Inscription" localSheetId="0">Inscription!$A$1:$M$427</definedName>
-    <definedName name="Inscription_Feature" localSheetId="4">'Inscription Feature'!$A$1:$E$636</definedName>
-    <definedName name="Inscription_Macroscopic" localSheetId="7">'Inscription Macroscopic'!$A$1:$K$680</definedName>
-    <definedName name="Inscription_Multistone" localSheetId="5">'Inscription Multistone'!$A$1:$C$30</definedName>
-    <definedName name="Inscription_Reference" localSheetId="6">'Inscription Reference'!$A$1:$E$503</definedName>
-    <definedName name="Institution" localSheetId="1">Institution!$A$1:$F$26</definedName>
-    <definedName name="Institution_Honor" localSheetId="9">'Institution Honor'!$A$1:$C$51</definedName>
-    <definedName name="Institution_Sponsorship" localSheetId="10">'Institution Sponsor'!$A$1:$E$226</definedName>
-    <definedName name="Person" localSheetId="2">Person!$A$1:$P$540</definedName>
-    <definedName name="Person_Honor_Display" localSheetId="12">'Person Honor Display'!$A$1:$E$518</definedName>
-    <definedName name="Person_in_Inscription" localSheetId="11">'Person in Inscription'!$A$1:$D$692</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -57,177 +42,8 @@
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{5AD6806A-D913-AD47-A67B-B94A94ED103D}" name="Honor" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Honor.csv" tab="0" comma="1">
-      <textFields count="6">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="2" xr16:uid="{13D600B9-EAEB-FE48-BB7C-0CAB5D8906D6}" name="Honor in Inscription" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Honor in Inscription.csv" tab="0" comma="1">
-      <textFields count="4">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="3" xr16:uid="{D4302EDB-5446-7540-979C-F3555943A962}" name="Inscription" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Inscription.csv" tab="0" comma="1">
-      <textFields count="13">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="4" xr16:uid="{A0E9CB3D-D84E-AD46-A205-AF1A00B4EBA3}" name="Inscription Feature" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Inscription Feature.csv" tab="0" comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="5" xr16:uid="{E48D42FC-C7AE-D946-82AC-63C5AD446A36}" name="Inscription Macroscopic" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Inscription Macroscopic.csv" tab="0" comma="1">
-      <textFields count="11">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="6" xr16:uid="{D38656E9-9B8C-EB45-B01A-DB653162EBD4}" name="Inscription Multistone" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Inscription Multistone.csv" tab="0" comma="1">
-      <textFields count="3">
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="7" xr16:uid="{6DFD4C03-2351-7049-81BB-1B72085CD6CF}" name="Inscription Reference" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Inscription Reference.csv" tab="0" comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="8" xr16:uid="{26F9DE31-FAFE-794F-9DDB-FC01601F1DE7}" name="Institution" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Institution.csv" tab="0" comma="1">
-      <textFields count="6">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="9" xr16:uid="{94D7AEF2-3632-8243-9C73-8A667556DCC3}" name="Institution Honor" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Institution Honor.csv" tab="0" comma="1">
-      <textFields count="3">
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="10" xr16:uid="{8F4AE480-E21A-644E-A1B2-2D18188511A6}" name="Institution Sponsorship" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Institution Sponsorship.csv" tab="0" comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="11" xr16:uid="{19B6F6C9-A03B-A04D-AC3B-024B0F03A092}" name="Person" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Person.csv" tab="0" comma="1">
-      <textFields count="16">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="12" xr16:uid="{C720D2F7-74A7-534C-853B-A0F201D988D3}" name="Person Honor Display" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Person Honor Display.csv" tab="0" comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="13" xr16:uid="{EAA83F49-05F2-FA4E-8EE2-F9C5A747955F}" name="Person in Inscription" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/davidthomas/Git/brown-diss/import_data/Person in Inscription.csv" tab="0" comma="1">
-      <textFields count="4">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12998" uniqueCount="2133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12998" uniqueCount="2134">
   <si>
     <t>ID</t>
   </si>
@@ -6626,6 +6442,9 @@
   </si>
   <si>
     <t>Honorand</t>
+  </si>
+  <si>
+    <t>ss</t>
   </si>
 </sst>
 </file>
@@ -6680,56 +6499,207 @@
 </styleSheet>
 </file>
 
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Inscription" connectionId="3" xr16:uid="{0E191096-E182-C348-B934-5E51EF8D5718}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA6A544B-D3BF-B547-B7C4-9FD0AB916D01}" name="Inscriptions" displayName="Inscriptions" ref="A1:M427" totalsRowShown="0">
+  <autoFilter ref="A1:M427" xr:uid="{C554A75D-81B4-CE4A-9AFF-EEF1CB75A31F}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{4F5AF829-1AC7-7342-A9D5-8CE5B23CC53E}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{6D24A295-08C6-394F-B60C-9DBA83FA601A}" name="IE"/>
+    <tableColumn id="3" xr3:uid="{356DDCF0-BB9B-6447-B405-D9EF92FA61C9}" name="Inscription"/>
+    <tableColumn id="4" xr3:uid="{0D1754CE-C3BD-C843-BB83-6B2F41C42AD7}" name="Object Type"/>
+    <tableColumn id="5" xr3:uid="{3A412424-FB2D-EF43-95FE-00032C9B8A50}" name="Inscription Type"/>
+    <tableColumn id="6" xr3:uid="{0068E214-3903-9A47-B10E-123FE0EE4A2E}" name="Location"/>
+    <tableColumn id="7" xr3:uid="{0D284548-1FBA-A947-9B66-D33E7A4918DD}" name="Low Date"/>
+    <tableColumn id="8" xr3:uid="{29A5B4D6-B6C1-A742-89FF-95313888CDBB}" name="High Date"/>
+    <tableColumn id="9" xr3:uid="{955FCDAF-B27F-E341-8B04-2312E8079634}" name="Date"/>
+    <tableColumn id="10" xr3:uid="{5B74AA76-9593-6F4F-B5A6-972768D5AB17}" name="Date Span"/>
+    <tableColumn id="11" xr3:uid="{67BF4EA4-3132-9041-951B-EB5631D70743}" name="Low Date Uncertain"/>
+    <tableColumn id="12" xr3:uid="{33BCFB75-54E4-164B-8656-A3E7A4DC99BB}" name="High Date Uncertain"/>
+    <tableColumn id="13" xr3:uid="{10A7224C-3082-754D-B82D-0DF480398FF6}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Institution Honor" connectionId="9" xr16:uid="{072F9D0A-B91F-A249-BC4E-EAE735E226CE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{3DF432E6-E607-4146-8DB3-778C848B8B76}" name="InstitutionHonor" displayName="InstitutionHonor" ref="A1:C51" totalsRowShown="0">
+  <autoFilter ref="A1:C51" xr:uid="{0F9E0EE6-0B8F-2442-9236-C131956A134C}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{67052DAC-B68C-1347-81BD-1D7F39E6ABB0}" name="Institution ID"/>
+    <tableColumn id="2" xr3:uid="{6B70E209-38B6-8F4A-8030-2DDE3C0BD628}" name="Honor ID"/>
+    <tableColumn id="3" xr3:uid="{89BBFEC6-5C58-FA44-9672-9809FA213DB8}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Institution Sponsorship" connectionId="10" xr16:uid="{AED64631-06F5-0245-A23F-703CB1E13DA7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{DFE2E066-AE53-3548-BFA9-46E997C63C98}" name="InstitutionSponsor" displayName="InstitutionSponsor" ref="A1:E226" totalsRowShown="0">
+  <autoFilter ref="A1:E226" xr:uid="{9D614BBC-07E0-AB4B-9F1A-C77688E9193B}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{4FE69899-64AA-CA4F-8DCF-42E1386834EF}" name="Institution ID"/>
+    <tableColumn id="2" xr3:uid="{1120EE57-3BC7-AC4A-B607-97B618421401}" name="Inscription ID"/>
+    <tableColumn id="3" xr3:uid="{571E4CCF-DB00-A746-83D0-BBEE924D5F9A}" name="Role"/>
+    <tableColumn id="4" xr3:uid="{67B01920-8408-A64B-B6D1-37073EAA0A14}" name="Uncertain"/>
+    <tableColumn id="5" xr3:uid="{3CD76B69-CB6B-DC4D-8BE9-722FBEA66BE5}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Person in Inscription" connectionId="13" xr16:uid="{99EE5CFD-9BEE-1948-AACB-E8107EE749AE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{6B1D9AB0-FFD6-AC41-A8FF-B7F274F103B4}" name="PersonInInscription" displayName="PersonInInscription" ref="A1:D692" totalsRowShown="0">
+  <autoFilter ref="A1:D692" xr:uid="{6D93D17B-E4D0-D54B-BE5A-130492433544}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FCBCD14E-DDF3-454D-A916-3FCABD4F86C7}" name="Person ID"/>
+    <tableColumn id="2" xr3:uid="{BC336BAE-6D9A-124B-8B38-C0501DE14C4C}" name="Inscription ID"/>
+    <tableColumn id="3" xr3:uid="{27699265-1E2A-E94F-BBB1-440FEDBE6BE5}" name="Role"/>
+    <tableColumn id="4" xr3:uid="{756BA270-7FA3-D34F-A32C-461C09527F86}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Person Honor Display" connectionId="12" xr16:uid="{4A19CF7C-96EB-1B4B-8F04-31B48A7E5858}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{0EB08918-3F3F-154B-95AE-2B6EC9A0521F}" name="PersonHonorDisplay" displayName="PersonHonorDisplay" ref="A1:E518" totalsRowShown="0">
+  <autoFilter ref="A1:E518" xr:uid="{EBA468DE-D4C2-BF48-AFD5-80D6F1EE99FB}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{4A416652-2FBD-8842-827F-7515B6747B7A}" name="Person ID"/>
+    <tableColumn id="2" xr3:uid="{643218A3-A153-F143-8823-52F217B9476D}" name="Honor ID"/>
+    <tableColumn id="3" xr3:uid="{FF63052D-8FB9-6240-9BD9-ED7E7E55BE56}" name="Inscription ID"/>
+    <tableColumn id="4" xr3:uid="{B84B1782-4BFD-F841-B76B-F473BC29B5E1}" name="Uncertain"/>
+    <tableColumn id="5" xr3:uid="{2840E39E-12EA-F54A-A70B-1E2605C9E1AA}" name="Appearances"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Institution" connectionId="8" xr16:uid="{C8807BBB-E08F-7542-9B58-626AB9F80277}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FD642A0B-C247-C74A-B5DA-F88267575C38}" name="Institutions" displayName="Institutions" ref="A1:F26" totalsRowShown="0">
+  <autoFilter ref="A1:F26" xr:uid="{AD630532-C26E-7747-B137-3AD08BF9FE24}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7C863CEA-3E92-C346-AD38-F6D4B2006C57}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{3AE89A32-131F-5445-8B27-1E3AE0E531D7}" name="Institution"/>
+    <tableColumn id="3" xr3:uid="{E5035A06-C0A6-CA48-99C4-A8FBFE08DB6E}" name="Origin"/>
+    <tableColumn id="4" xr3:uid="{F090621E-6243-5747-AB17-7D5E6CC08C19}" name="Type"/>
+    <tableColumn id="5" xr3:uid="{A06582C5-7D7D-8D4F-A4E6-24919212EE1D}" name="Category"/>
+    <tableColumn id="6" xr3:uid="{2AD0656F-35DC-4F4A-A0C9-01FED456E181}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Person" connectionId="11" xr16:uid="{B95E6B55-713F-9A4A-A15E-BC2AD6A04F3B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A932EFEA-769E-6741-AF94-FAC50E1882F9}" name="People" displayName="People" ref="A1:P540" totalsRowShown="0">
+  <autoFilter ref="A1:P540" xr:uid="{F005076A-8E8E-3B4C-9F02-0C4F9313D8B6}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{9C6C46A7-2F84-4E43-8620-84DB6C74F2F9}" name="ss"/>
+    <tableColumn id="2" xr3:uid="{515E5A13-6935-E441-B0A6-13387AE6A9E6}" name="Person"/>
+    <tableColumn id="3" xr3:uid="{40A5FA94-3CD6-C546-8FEC-69B957E1498F}" name="Category"/>
+    <tableColumn id="4" xr3:uid="{682C165A-E39D-F446-888A-D77FD1D2CFCE}" name="Origin"/>
+    <tableColumn id="5" xr3:uid="{65A40C60-366E-2C4C-9B34-BFEA118CDF88}" name="Gender"/>
+    <tableColumn id="6" xr3:uid="{12AA5A54-115A-6B4D-89F0-41035B76E1EF}" name="Athenian Citizen"/>
+    <tableColumn id="7" xr3:uid="{B4CCA97A-122B-F84B-99A8-0752A94BBD2B}" name="Roman Citizen"/>
+    <tableColumn id="8" xr3:uid="{44F77901-18D2-4047-8C4B-C02CAEF4F013}" name="Family"/>
+    <tableColumn id="9" xr3:uid="{901A703E-B538-5D40-ACB7-B8090070BC4E}" name="Extended"/>
+    <tableColumn id="10" xr3:uid="{EF5D740D-6C12-C549-957A-2C0DC883FFB9}" name="Praenomen"/>
+    <tableColumn id="11" xr3:uid="{3FA27551-4BEE-3041-B4BB-5185B42E2DFA}" name="Nomen"/>
+    <tableColumn id="12" xr3:uid="{0DC31EE8-2434-6D43-9044-C1094A691920}" name="Cognomen"/>
+    <tableColumn id="13" xr3:uid="{77EEE78C-CE87-7142-A343-4ACF46EA813A}" name="Onomos"/>
+    <tableColumn id="14" xr3:uid="{D0F5B3E5-52BE-494F-BC6E-6D72B318BEC6}" name="Patronym"/>
+    <tableColumn id="15" xr3:uid="{076C4154-33D0-7F4B-BA6D-7F70FF32E98D}" name="Deme"/>
+    <tableColumn id="16" xr3:uid="{C2703CB2-FF25-D547-ADFF-DF51388C593E}" name="Uncertain Person"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Honor" connectionId="1" xr16:uid="{B26F8A15-C0AA-DD43-9C1E-7ADDB39DEB11}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A5841345-B13A-D040-8093-E217FA8FAF08}" name="Honors" displayName="Honors" ref="A1:F141" totalsRowShown="0">
+  <autoFilter ref="A1:F141" xr:uid="{626A3160-AB3F-624A-944D-EE8DA5F528EF}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8413FBA6-0795-2F4B-B856-DA63911B5D58}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{92F75BF5-89BC-2642-B2B0-6EF99F6BE345}" name="Honor"/>
+    <tableColumn id="3" xr3:uid="{EDC8B7E2-8915-0447-A19E-735B12A70D91}" name="Origin"/>
+    <tableColumn id="4" xr3:uid="{8C12598A-4C2C-A84D-B639-C7AAC488B45F}" name="Category"/>
+    <tableColumn id="5" xr3:uid="{9452ABAD-6766-A443-8DAF-C8D938B7BB0A}" name="Type"/>
+    <tableColumn id="6" xr3:uid="{C9B9DE4A-1123-2741-84E5-73D1B5BF26DA}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Inscription Feature" connectionId="4" xr16:uid="{7A05516B-B9ED-024B-82E9-8FB9174098ED}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BB5E3213-12A9-C642-98AD-FF8D4E55E32A}" name="InscriptionFeature" displayName="InscriptionFeature" ref="A1:E636" totalsRowShown="0">
+  <autoFilter ref="A1:E636" xr:uid="{6E0CC81D-80A6-A04E-B3D8-1ADFB655C09F}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{946C41D8-EFC3-7349-A47E-A11A8AF5BDE5}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{5C868747-FD17-2B42-96ED-CA2BB4C3DD8D}" name="Inscription ID"/>
+    <tableColumn id="3" xr3:uid="{49A48574-5EDD-4A40-8B7F-BD90B57EDC2A}" name="Feature"/>
+    <tableColumn id="4" xr3:uid="{8D170D4C-A351-4F45-9264-E612AE167C54}" name="Uncertain"/>
+    <tableColumn id="5" xr3:uid="{ECF38C63-38F0-E14A-91F3-13522E275A1D}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Inscription Multistone" connectionId="6" xr16:uid="{A488F7DA-0FCA-7246-9539-BD11C14031C4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FDAF7FF7-8662-F84C-B0FD-9A26787520B0}" name="InscriptionMultistone" displayName="InscriptionMultistone" ref="A1:C30" totalsRowShown="0">
+  <autoFilter ref="A1:C30" xr:uid="{F7CFA075-BA08-8645-ABAC-6558A96672C7}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6CA54BAB-3A04-9C48-9C0A-C7362856B4DB}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{D39516D3-66E4-F049-9E3B-64FB64C1553B}" name="IE"/>
+    <tableColumn id="3" xr3:uid="{BDE8579E-1DC8-1E44-A6CB-46872F2A60B7}" name="Part"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Inscription Reference" connectionId="7" xr16:uid="{21E86C10-377E-C049-84A7-1DE3615320B5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9CA6A10B-410E-5B4F-8F08-099B0AF6F053}" name="InscriptionReference" displayName="InscriptionReference" ref="A1:E503" totalsRowShown="0">
+  <autoFilter ref="A1:E503" xr:uid="{4D3CCDE3-9D61-DF42-B8AA-420C0D56550A}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{373CB0CD-5D62-574A-9B98-3F568EEA01CC}" name="Inscription ID"/>
+    <tableColumn id="2" xr3:uid="{49C1AD0F-96D1-F249-BE5F-746465AFF36A}" name="Publication"/>
+    <tableColumn id="3" xr3:uid="{ABB1FD34-495D-7449-8824-E2079D02F7B9}" name="Number"/>
+    <tableColumn id="4" xr3:uid="{3CD04EFB-11C9-CF4A-832C-9FC6092E72B7}" name="Additional"/>
+    <tableColumn id="5" xr3:uid="{ADCBA1D9-D5B5-634F-A4FF-EF4E38CE29B3}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Inscription Macroscopic" connectionId="5" xr16:uid="{97525CB8-8D9A-F146-BE56-D0B1E9CD788F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4B753879-4AD8-CC42-B725-F3251A932D33}" name="InscriptionMacroscopic" displayName="InscriptionMacroscopic" ref="A1:K680" totalsRowShown="0">
+  <autoFilter ref="A1:K680" xr:uid="{BAE8668F-BF5F-6D4B-BF44-EAD6B443170D}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{EDB0A9E4-3CD3-BA40-807E-548D37486DE2}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{D6F5AF9A-5EFE-E94B-A539-501A620D0849}" name="Inscription"/>
+    <tableColumn id="3" xr3:uid="{9D37D0FC-12D8-4F40-B0C1-BFCAA246B8C9}" name="Date"/>
+    <tableColumn id="4" xr3:uid="{B760D961-31D9-344A-A794-9C7DDCDCED91}" name="Date Strength"/>
+    <tableColumn id="5" xr3:uid="{1CE03369-73C7-D841-936D-2DEB6A11309E}" name="Inscription Type"/>
+    <tableColumn id="6" xr3:uid="{44957DF3-CDA8-AF4B-A378-4B123D67E005}" name="Object Type"/>
+    <tableColumn id="7" xr3:uid="{3F0849A2-5FBB-7049-9D38-ED326F343B3E}" name="Altered"/>
+    <tableColumn id="8" xr3:uid="{BFEC1207-A355-5747-92B8-E38E86F5C814}" name="Visuals"/>
+    <tableColumn id="9" xr3:uid="{9BD27271-C083-5F49-8B25-8EF8A4638615}" name="Text Format"/>
+    <tableColumn id="10" xr3:uid="{CC655641-F74B-AA40-8183-00EA59AB6E2B}" name="Sponsor Type"/>
+    <tableColumn id="11" xr3:uid="{9DBE318E-406F-8D4F-BAD3-03C2021AD04D}" name="Honorand Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Honor in Inscription" connectionId="2" xr16:uid="{CF7E3762-72A5-E64D-A312-C6918F591228}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{3CA04679-7137-1046-9C5D-316C2322EF8D}" name="HonorInInscription" displayName="HonorInInscription" ref="A1:D492" totalsRowShown="0">
+  <autoFilter ref="A1:D492" xr:uid="{717B910A-7E63-D640-8DF5-39F33033EB4F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{82F50351-E3BA-BF4D-8AB2-9154ECEF426F}" name="Honor ID"/>
+    <tableColumn id="2" xr3:uid="{1FB8719D-F83D-C843-B4AA-BFCBD7500E2F}" name="Inscription ID"/>
+    <tableColumn id="3" xr3:uid="{0A00535F-B962-EC42-BA7C-DFF8790BD98C}" name="Appearances"/>
+    <tableColumn id="4" xr3:uid="{7D72ACD0-FB90-ED4F-BB87-C5FCDEC94EBE}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7031,24 +7001,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E1310E-F434-2F40-A573-F04EA3F9AC57}">
   <dimension ref="A1:M427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="80.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -22256,6 +22227,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -22263,13 +22237,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1359A1E-2378-F645-877F-EE4E9F65DF55}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -22685,6 +22661,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -22692,15 +22671,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6699D2EB-E3FC-C74D-B248-5F8EC4026096}">
   <dimension ref="A1:E226"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E226"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -25872,6 +25853,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -25879,14 +25863,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF07D02D-A550-444D-B33B-F0F6FE82FC03}">
   <dimension ref="A1:D692"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D692"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -32342,6 +32328,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -32349,15 +32338,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C3925E-877F-D94D-AA56-411C31695634}">
   <dimension ref="A1:E518"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -41168,6 +41159,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -41175,16 +41169,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CBF3A7-56AC-274C-B988-DCEE9D0AAE9D}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -41634,6 +41630,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -41641,7 +41640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1E3B16-F8C6-F244-92EE-71CDCA2E25C0}">
   <dimension ref="A1:P540"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P540"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -41649,22 +41650,22 @@
     <col min="2" max="2" width="37.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="9" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2133</v>
       </c>
       <c r="B1" t="s">
         <v>1080</v>
@@ -59724,6 +59725,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -59731,15 +59735,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95D3DA6-E790-C94A-B696-5C0EB7504532}">
   <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F141"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -62144,6 +62151,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -62151,15 +62161,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBE968E-1BE2-D940-8B1C-895A8F1699D8}">
   <dimension ref="A1:E636"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E636"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -69181,6 +69193,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -69188,12 +69203,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B43054D-4171-B247-821D-7B3C383C0414}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -69528,6 +69546,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -69535,15 +69556,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FD5817-BB38-7644-B790-C3B4EA463FC0}">
   <dimension ref="A1:E503"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E503"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -75186,6 +75209,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -75193,21 +75219,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A50DD13C-7FAD-2645-86D2-AF484B460C35}">
   <dimension ref="A1:K680"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="80.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -92883,6 +92911,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -92890,14 +92921,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81014F09-C73C-1642-B72E-2181D9308636}">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D492"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -98317,5 +98350,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ie503 object type fixed to statue base
</commit_message>
<xml_diff>
--- a/eleusis_master.xlsx
+++ b/eleusis_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidthomas/Git/brown-diss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19514AE1-6108-6741-A801-8ED774899DB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DD6FEC-B58A-5944-952E-358CBB5037C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="12" xr2:uid="{0C2D7FDC-D2BD-754C-9966-FCA1A3DC457F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0C2D7FDC-D2BD-754C-9966-FCA1A3DC457F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inscription" sheetId="1" r:id="rId1"/>
@@ -7001,8 +7001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E1310E-F434-2F40-A573-F04EA3F9AC57}">
   <dimension ref="A1:M427"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M427"/>
+    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
+      <selection activeCell="D257" sqref="D257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16117,7 +16117,7 @@
         <v>234</v>
       </c>
       <c r="D256" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="E256" t="s">
         <v>15</v>
@@ -32338,7 +32338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C3925E-877F-D94D-AA56-411C31695634}">
   <dimension ref="A1:E518"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
person column id typo fixed
</commit_message>
<xml_diff>
--- a/eleusis_master.xlsx
+++ b/eleusis_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidthomas/Git/brown-diss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DD6FEC-B58A-5944-952E-358CBB5037C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502D4E1A-8F5C-3E43-8148-5CC4C9060599}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0C2D7FDC-D2BD-754C-9966-FCA1A3DC457F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{0C2D7FDC-D2BD-754C-9966-FCA1A3DC457F}"/>
   </bookViews>
   <sheets>
     <sheet name="Inscription" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12998" uniqueCount="2134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12998" uniqueCount="2133">
   <si>
     <t>ID</t>
   </si>
@@ -6442,9 +6442,6 @@
   </si>
   <si>
     <t>Honorand</t>
-  </si>
-  <si>
-    <t>ss</t>
   </si>
 </sst>
 </file>
@@ -6593,7 +6590,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A932EFEA-769E-6741-AF94-FAC50E1882F9}" name="People" displayName="People" ref="A1:P540" totalsRowShown="0">
   <autoFilter ref="A1:P540" xr:uid="{F005076A-8E8E-3B4C-9F02-0C4F9313D8B6}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{9C6C46A7-2F84-4E43-8620-84DB6C74F2F9}" name="ss"/>
+    <tableColumn id="1" xr3:uid="{9C6C46A7-2F84-4E43-8620-84DB6C74F2F9}" name="ID"/>
     <tableColumn id="2" xr3:uid="{515E5A13-6935-E441-B0A6-13387AE6A9E6}" name="Person"/>
     <tableColumn id="3" xr3:uid="{40A5FA94-3CD6-C546-8FEC-69B957E1498F}" name="Category"/>
     <tableColumn id="4" xr3:uid="{682C165A-E39D-F446-888A-D77FD1D2CFCE}" name="Origin"/>
@@ -7001,7 +6998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E1310E-F434-2F40-A573-F04EA3F9AC57}">
   <dimension ref="A1:M427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
+    <sheetView topLeftCell="A242" workbookViewId="0">
       <selection activeCell="D257" sqref="D257"/>
     </sheetView>
   </sheetViews>
@@ -41640,8 +41637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1E3B16-F8C6-F244-92EE-71CDCA2E25C0}">
   <dimension ref="A1:P540"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P540"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41665,7 +41662,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2133</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1080</v>

</xml_diff>